<commit_message>
test faster record image
</commit_message>
<xml_diff>
--- a/static/server_activities_log.xlsx
+++ b/static/server_activities_log.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="126" uniqueCount="37">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="129" uniqueCount="38">
   <si>
     <t>Login</t>
   </si>
@@ -125,6 +125,9 @@
   </si>
   <si>
     <t>06/05/2022 09:29:29 PM</t>
+  </si>
+  <si>
+    <t>07/05/2022 03:29:56 AM</t>
   </si>
 </sst>
 </file>
@@ -456,7 +459,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D42"/>
+  <dimension ref="A1:D43"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1050,6 +1053,20 @@
         <v>36</v>
       </c>
     </row>
+    <row r="43" spans="1:4">
+      <c r="A43">
+        <v>43</v>
+      </c>
+      <c r="B43" t="s">
+        <v>0</v>
+      </c>
+      <c r="C43" t="s">
+        <v>1</v>
+      </c>
+      <c r="D43" t="s">
+        <v>37</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
modified chart.js responsiveness on mobile
</commit_message>
<xml_diff>
--- a/static/server_activities_log.xlsx
+++ b/static/server_activities_log.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="45">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="46">
   <si>
     <t>Login</t>
   </si>
@@ -149,6 +149,9 @@
   </si>
   <si>
     <t>09/05/2022 02:31:17 AM</t>
+  </si>
+  <si>
+    <t>09/05/2022 03:20:46 AM</t>
   </si>
 </sst>
 </file>
@@ -480,7 +483,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D51"/>
+  <dimension ref="A1:D52"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1200,6 +1203,20 @@
         <v>44</v>
       </c>
     </row>
+    <row r="52" spans="1:4">
+      <c r="A52">
+        <v>52</v>
+      </c>
+      <c r="B52" t="s">
+        <v>0</v>
+      </c>
+      <c r="C52" t="s">
+        <v>1</v>
+      </c>
+      <c r="D52" t="s">
+        <v>45</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
chnaged end device 1 location to nottingham
</commit_message>
<xml_diff>
--- a/static/server_activities_log.xlsx
+++ b/static/server_activities_log.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="156" uniqueCount="46">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="159" uniqueCount="47">
   <si>
     <t>Login</t>
   </si>
@@ -152,6 +152,9 @@
   </si>
   <si>
     <t>09/05/2022 03:20:46 AM</t>
+  </si>
+  <si>
+    <t>09/05/2022 10:25:20 AM</t>
   </si>
 </sst>
 </file>
@@ -483,7 +486,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D52"/>
+  <dimension ref="A1:D53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -1217,6 +1220,20 @@
         <v>45</v>
       </c>
     </row>
+    <row r="53" spans="1:4">
+      <c r="A53">
+        <v>53</v>
+      </c>
+      <c r="B53" t="s">
+        <v>0</v>
+      </c>
+      <c r="C53" t="s">
+        <v>1</v>
+      </c>
+      <c r="D53" t="s">
+        <v>46</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>